<commit_message>
House Prices Prediction Project
</commit_message>
<xml_diff>
--- a/House_Price_Prediction/plan_regression.xlsx
+++ b/House_Price_Prediction/plan_regression.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ara/House_Price_Project_X/Modeling_byaracho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ara/Kaggle_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="11760" yWindow="800" windowWidth="21360" windowHeight="14180" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
-    <sheet name="시트3" sheetId="3" r:id="rId2"/>
-    <sheet name="시트2" sheetId="2" r:id="rId3"/>
+    <sheet name="시트5" sheetId="7" r:id="rId2"/>
+    <sheet name="시트3" sheetId="3" r:id="rId3"/>
+    <sheet name="시트2" sheetId="2" r:id="rId4"/>
+    <sheet name="시트6" sheetId="6" r:id="rId5"/>
+    <sheet name="시트4" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="215">
   <si>
     <t>cook's distance</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -636,12 +639,276 @@
     <t>leverage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>variable select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기준</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>갯수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제외한 칼럼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제외한 이유</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotRmsAbvGrd, Yearsold, YearRemodAdd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIF Factor와 상관관계 고려</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GarageArea, GarageYrBlt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*위에서 제외한 칼럼 다시 제외</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_1의 VIF factor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_4의 VIF factor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>numerical feature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>categorical feature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_c2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test 데이터에 없는 더미 클래스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상관계수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PoolQC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condition2, RoofMatl, Functional</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_c3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(select_2 | select_3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t-test p_value &lt; 0.005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t-test p_value &lt; 0.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(select_c1 | select_c2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adj rsquared</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ill No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kaggle 제출 결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2)numerical + categorical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1)numerical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_5 + c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PoolArea, 1stFlrArea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rmse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Cond. No. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_1 + c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_1 + c2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_1 + c3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leverage &gt; 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leverage | cook's</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leverage | cook's | IQR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>68개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none값이 많음, scale 불가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outliers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2개(dummies 28개)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4개(dummies 34개)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5개(dummies 38개)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rsquared_adj</t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>Model 1-1</t>
+  </si>
+  <si>
+    <t>Model 1-2</t>
+  </si>
+  <si>
+    <t>Model 1-3</t>
+  </si>
+  <si>
+    <t>Model 1-4</t>
+  </si>
+  <si>
+    <t>Model 1-5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -797,8 +1064,61 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,8 +1131,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -930,15 +1262,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1004,13 +1364,64 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="기본" xfId="0" builtinId="0"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="하이퍼링크" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1287,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A25" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -1786,10 +2197,113 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="4" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="63"/>
+      <c r="B1" s="64" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="61">
+        <v>0.99984767900000004</v>
+      </c>
+      <c r="C2" s="62">
+        <v>-1393.3948800000001</v>
+      </c>
+      <c r="D2" s="61">
+        <v>-1218.9505529999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="59">
+        <v>0.86167986500000004</v>
+      </c>
+      <c r="C3" s="59">
+        <v>-1214.717316</v>
+      </c>
+      <c r="D3" s="59">
+        <v>1.1067779870000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="59">
+        <v>0.93322646200000003</v>
+      </c>
+      <c r="C4" s="58">
+        <v>-2251.6884759999998</v>
+      </c>
+      <c r="D4" s="59">
+        <v>-861.42005470000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" s="59">
+        <v>0.99981677599999996</v>
+      </c>
+      <c r="C5" s="59">
+        <v>-1142.3929659999999</v>
+      </c>
+      <c r="D5" s="59">
+        <v>-1068.3862819999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="65" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="59">
+        <v>0.86701050000000002</v>
+      </c>
+      <c r="C6" s="59">
+        <v>-1430.768358</v>
+      </c>
+      <c r="D6" s="59">
+        <v>-1155.886389</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -1967,15 +2481,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2359,5 +2874,783 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="11" max="13" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="41">
+        <v>0.99986770390929602</v>
+      </c>
+      <c r="D3" s="41">
+        <v>-1571.41148024319</v>
+      </c>
+      <c r="E3" s="41">
+        <v>-1392.2918975237601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0.99992930688714998</v>
+      </c>
+      <c r="D4" s="41">
+        <v>-2396.2177042866902</v>
+      </c>
+      <c r="E4" s="41">
+        <v>-2223.3236101519501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="49">
+        <v>0.99993378958238199</v>
+      </c>
+      <c r="D5" s="49">
+        <v>-2470.1820540334602</v>
+      </c>
+      <c r="E5" s="49">
+        <v>-2297.5257130885202</v>
+      </c>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="41">
+        <v>0.99989134134266999</v>
+      </c>
+      <c r="D6" s="41">
+        <v>-1824.7289480357999</v>
+      </c>
+      <c r="E6" s="41">
+        <v>-1646.18321860115</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="41">
+        <v>0.99993451374204101</v>
+      </c>
+      <c r="D7" s="41">
+        <v>-2419.4504149998802</v>
+      </c>
+      <c r="E7" s="41">
+        <v>-2247.71348836269</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="H8" s="35"/>
+    </row>
+    <row r="11" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="G11" s="35"/>
+      <c r="I11" s="33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="G12" s="35"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="K12" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="L12" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="M12" s="50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="G13" s="35"/>
+      <c r="I13" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="K13" s="41">
+        <v>0.99986770390929602</v>
+      </c>
+      <c r="L13" s="41">
+        <v>-1571.41148024319</v>
+      </c>
+      <c r="M13" s="41">
+        <v>-1392.2918975237601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I14" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="K14" s="41">
+        <v>0.99992930688714998</v>
+      </c>
+      <c r="L14" s="41">
+        <v>-2396.2177042866902</v>
+      </c>
+      <c r="M14" s="41">
+        <v>-2223.3236101519501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I15" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="J15" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="K15" s="49">
+        <v>0.99993378958238199</v>
+      </c>
+      <c r="L15" s="49">
+        <v>-2470.1820540334602</v>
+      </c>
+      <c r="M15" s="49">
+        <v>-2297.5257130885202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I16" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="K16" s="41">
+        <v>0.99989134134266999</v>
+      </c>
+      <c r="L16" s="41">
+        <v>-1824.7289480357999</v>
+      </c>
+      <c r="M16" s="41">
+        <v>-1646.18321860115</v>
+      </c>
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I17" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>202</v>
+      </c>
+      <c r="K17" s="41">
+        <v>0.99993451374204101</v>
+      </c>
+      <c r="L17" s="41">
+        <v>-2419.4504149998802</v>
+      </c>
+      <c r="M17" s="41">
+        <v>-2247.71348836269</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="53"/>
+      <c r="B10" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="42"/>
+      <c r="B17" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="48">
+        <v>0.91175208039948497</v>
+      </c>
+      <c r="C18" s="48">
+        <v>-2139.2885869151401</v>
+      </c>
+      <c r="D18" s="48">
+        <v>-2034.6194785427101</v>
+      </c>
+      <c r="E18" s="48">
+        <v>6.12</v>
+      </c>
+      <c r="F18" s="48">
+        <v>23458.841351468101</v>
+      </c>
+      <c r="G18" s="48">
+        <v>0.14201</v>
+      </c>
+      <c r="H18" s="44"/>
+      <c r="I18" s="29"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="41">
+        <v>0.906240514919332</v>
+      </c>
+      <c r="C19" s="41">
+        <v>-2059.32885737588</v>
+      </c>
+      <c r="D19" s="41">
+        <v>-1975.5935706779401</v>
+      </c>
+      <c r="E19" s="41">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F19" s="41">
+        <v>24158.4036333533</v>
+      </c>
+      <c r="G19" s="41">
+        <v>0.14440800000000001</v>
+      </c>
+      <c r="H19" s="44"/>
+      <c r="I19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="41">
+        <v>0.86715980043216101</v>
+      </c>
+      <c r="C20" s="41">
+        <v>-1580.7345285276799</v>
+      </c>
+      <c r="D20" s="41">
+        <v>-1517.9330635042299</v>
+      </c>
+      <c r="E20" s="41">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="F20" s="41">
+        <v>27157.2055500118</v>
+      </c>
+      <c r="G20" s="41"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="29"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="41">
+        <v>0.90916931221956299</v>
+      </c>
+      <c r="C21" s="41">
+        <v>-2100.3211032811901</v>
+      </c>
+      <c r="D21" s="41">
+        <v>-2000.8854503273801</v>
+      </c>
+      <c r="E21" s="41">
+        <v>20.6</v>
+      </c>
+      <c r="F21" s="41">
+        <v>23478.3176716979</v>
+      </c>
+      <c r="G21" s="41">
+        <v>0.14387</v>
+      </c>
+      <c r="H21" s="44"/>
+      <c r="I21" s="29"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="41">
+        <v>0.90635281264714496</v>
+      </c>
+      <c r="C22" s="41">
+        <v>-2060.00075256124</v>
+      </c>
+      <c r="D22" s="41">
+        <v>-1971.03201044467</v>
+      </c>
+      <c r="E22" s="41">
+        <v>4.76</v>
+      </c>
+      <c r="F22" s="41">
+        <v>24082.210784946099</v>
+      </c>
+      <c r="G22" s="41">
+        <v>0.14382</v>
+      </c>
+      <c r="H22" s="44"/>
+      <c r="I22" s="29"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I23" s="29"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="I24" s="29"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="47">
+        <v>0.94112503336775799</v>
+      </c>
+      <c r="C26" s="47">
+        <v>-2666.7804518825101</v>
+      </c>
+      <c r="D26" s="47">
+        <v>-2384.1738592769502</v>
+      </c>
+      <c r="E26" s="47">
+        <v>116</v>
+      </c>
+      <c r="F26" s="47">
+        <v>17513.471846654898</v>
+      </c>
+      <c r="G26" s="47">
+        <v>0.1245</v>
+      </c>
+      <c r="H26" s="46"/>
+      <c r="I26" s="29"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="B27" s="47">
+        <v>0.93148452844365404</v>
+      </c>
+      <c r="C27" s="47">
+        <v>-2468.2963332342902</v>
+      </c>
+      <c r="D27" s="47">
+        <v>-2217.1598373143802</v>
+      </c>
+      <c r="E27" s="41">
+        <v>114</v>
+      </c>
+      <c r="F27" s="47">
+        <v>20161.464390781301</v>
+      </c>
+      <c r="G27" s="41"/>
+      <c r="I27" s="29"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="B28" s="49">
+        <v>0.94220187772168895</v>
+      </c>
+      <c r="C28" s="49">
+        <v>-2693.9477330765699</v>
+      </c>
+      <c r="D28" s="49">
+        <v>-2390.4911338400202</v>
+      </c>
+      <c r="E28" s="49">
+        <v>124</v>
+      </c>
+      <c r="F28" s="49">
+        <v>17515.3191436325</v>
+      </c>
+      <c r="G28" s="49">
+        <v>0.12382</v>
+      </c>
+      <c r="I28" s="29"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" s="41">
+        <v>0.94021728114787495</v>
+      </c>
+      <c r="C29" s="41">
+        <v>-2648.4708497697402</v>
+      </c>
+      <c r="D29" s="41">
+        <v>-2381.5646234200399</v>
+      </c>
+      <c r="E29" s="41">
+        <v>108</v>
+      </c>
+      <c r="F29" s="41">
+        <v>17630.544674784302</v>
+      </c>
+      <c r="G29" s="41">
+        <v>0.12467</v>
+      </c>
+      <c r="H29" s="44"/>
+      <c r="I29" s="29"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" s="41">
+        <v>0.94125947551302103</v>
+      </c>
+      <c r="C30" s="55">
+        <v>-2674.4519099937802</v>
+      </c>
+      <c r="D30" s="55">
+        <v>-2386.6913417522201</v>
+      </c>
+      <c r="E30" s="47">
+        <v>115</v>
+      </c>
+      <c r="F30" s="55">
+        <v>17647.073069446102</v>
+      </c>
+      <c r="G30" s="41"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="29"/>
+    </row>
+    <row r="31" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="K31" s="35"/>
+    </row>
+    <row r="32" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="K32" s="35"/>
+    </row>
+    <row r="33" spans="7:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="G33" s="35"/>
+      <c r="K33" s="35"/>
+    </row>
+    <row r="34" spans="7:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="G34" s="35"/>
+    </row>
+    <row r="35" spans="7:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="G35" s="35"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>